<commit_message>
paee to paae en registros
</commit_message>
<xml_diff>
--- a/Datos/horarioactual.xlsx
+++ b/Datos/horarioactual.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,25 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17F43A95-307A-449E-9564-94AD238A65E9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB688670-D72D-4D9C-80EB-294261463F82}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{2DF8DE7C-993A-4A6D-9B6B-A57941C0789D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="horarioactual" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>idhorario</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -34,16 +37,316 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -51,15 +354,204 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -370,13 +862,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13A5B800-7921-4A6B-8760-E856C8046D0F}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
datos para login y horarios
</commit_message>
<xml_diff>
--- a/Datos/horarioactual.xlsx
+++ b/Datos/horarioactual.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\GitHub\iso\proyecto\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB688670-D72D-4D9C-80EB-294261463F82}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95069388-193C-4088-BF98-90E17CCD7060}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="horarioactual" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -862,10 +862,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A311"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A291" workbookViewId="0">
+      <selection activeCell="A300" sqref="A300"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -904,6 +906,1526 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>